<commit_message>
UI improvements Added the ability to havbe smaller maps than tile pieces (for map symmetry)
</commit_message>
<xml_diff>
--- a/Information.xlsx
+++ b/Information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Projects\CatanRandomizer\catan-randomizer-extreme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC20162-3617-4FD8-ADAF-FE26C0CBFD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BEEAFF-A79A-4288-8519-8BD203D95D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{6A0142DC-D103-449E-9AB9-8C7DD3A079BE}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" firstSheet="7" activeTab="11" xr2:uid="{6A0142DC-D103-449E-9AB9-8C7DD3A079BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tile Counts" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Triple Wide" sheetId="10" r:id="rId9"/>
     <sheet name="Exp Triple Wide" sheetId="11" r:id="rId10"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId11"/>
+    <sheet name="Double Peanut (2)" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -133,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="49">
   <si>
     <t>Desert</t>
   </si>
@@ -4547,12 +4548,1771 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871913AE-0291-453E-808C-A728D22CA13D}">
+  <dimension ref="A1:O107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="15" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="6">
+        <v>7</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16">
+        <v>27</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="6">
+        <v>6</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16">
+        <v>23</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16">
+        <v>32</v>
+      </c>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17">
+        <v>17</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17">
+        <v>28</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="16">
+        <v>36</v>
+      </c>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17">
+        <v>24</v>
+      </c>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17">
+        <v>33</v>
+      </c>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="6">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17">
+        <v>18</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17">
+        <v>29</v>
+      </c>
+      <c r="L8" s="18"/>
+      <c r="M8" s="16">
+        <v>37</v>
+      </c>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17">
+        <v>25</v>
+      </c>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17">
+        <v>34</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17">
+        <v>8</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17">
+        <v>19</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17">
+        <v>30</v>
+      </c>
+      <c r="L10" s="18"/>
+      <c r="M10" s="16">
+        <v>38</v>
+      </c>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17">
+        <v>4</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17">
+        <v>13</v>
+      </c>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17">
+        <v>26</v>
+      </c>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17">
+        <v>35</v>
+      </c>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17">
+        <v>9</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17">
+        <v>20</v>
+      </c>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17">
+        <v>31</v>
+      </c>
+      <c r="L12" s="18"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="6">
+        <v>-2</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17">
+        <v>5</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17">
+        <v>14</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="6">
+        <v>-3</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17">
+        <v>2</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17">
+        <v>10</v>
+      </c>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17">
+        <v>21</v>
+      </c>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="6">
+        <v>-4</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17">
+        <v>6</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17">
+        <v>15</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="6">
+        <v>-5</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17">
+        <v>3</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17">
+        <v>11</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17">
+        <v>22</v>
+      </c>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="6">
+        <v>-6</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17">
+        <v>7</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17">
+        <v>16</v>
+      </c>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="6">
+        <v>-7</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18">
+        <v>12</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="6">
+        <v>-8</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="6">
+        <v>-12</v>
+      </c>
+      <c r="D20" s="6">
+        <v>-10</v>
+      </c>
+      <c r="E20" s="6">
+        <v>-8</v>
+      </c>
+      <c r="F20" s="6">
+        <v>-6</v>
+      </c>
+      <c r="G20" s="6">
+        <v>-4</v>
+      </c>
+      <c r="H20" s="6">
+        <v>-2</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6">
+        <v>2</v>
+      </c>
+      <c r="K20" s="6">
+        <v>4</v>
+      </c>
+      <c r="L20" s="6">
+        <v>6</v>
+      </c>
+      <c r="M20" s="6">
+        <v>8</v>
+      </c>
+      <c r="N20" s="6">
+        <v>10</v>
+      </c>
+      <c r="O20" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="C21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" cm="1">
+        <f t="array" ref="B24">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A24)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-8</v>
+      </c>
+      <c r="C24" cm="1">
+        <f t="array" ref="C24">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A24)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-1</v>
+      </c>
+      <c r="D24" t="str">
+        <f>_xlfn.CONCAT("[",B24,", ",C24,"],")</f>
+        <v>[-8, -1],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" cm="1">
+        <f t="array" ref="B25">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A25)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-8</v>
+      </c>
+      <c r="C25" cm="1">
+        <f t="array" ref="C25">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A25)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-3</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" ref="D25:D88" si="0">_xlfn.CONCAT("[",B25,", ",C25,"],")</f>
+        <v>[-8, -3],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" cm="1">
+        <f t="array" ref="B26">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A26)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-8</v>
+      </c>
+      <c r="C26" cm="1">
+        <f t="array" ref="C26">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A26)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-5</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>[-8, -5],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" cm="1">
+        <f t="array" ref="B27">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A27)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-6</v>
+      </c>
+      <c r="C27" cm="1">
+        <f t="array" ref="C27">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A27)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>[-6, 0],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" cm="1">
+        <f t="array" ref="B28">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A28)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-6</v>
+      </c>
+      <c r="C28" cm="1">
+        <f t="array" ref="C28">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A28)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-2</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>[-6, -2],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" cm="1">
+        <f t="array" ref="B29">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A29)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-6</v>
+      </c>
+      <c r="C29" cm="1">
+        <f t="array" ref="C29">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A29)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-4</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>[-6, -4],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30" cm="1">
+        <f t="array" ref="B30">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A30)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-6</v>
+      </c>
+      <c r="C30" cm="1">
+        <f t="array" ref="C30">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A30)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-6</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>[-6, -6],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31" cm="1">
+        <f t="array" ref="B31">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A31)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-4</v>
+      </c>
+      <c r="C31" cm="1">
+        <f t="array" ref="C31">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A31)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>1</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>[-4, 1],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32" cm="1">
+        <f t="array" ref="B32">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A32)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-4</v>
+      </c>
+      <c r="C32" cm="1">
+        <f t="array" ref="C32">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A32)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-1</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>[-4, -1],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33" cm="1">
+        <f t="array" ref="B33">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A33)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-4</v>
+      </c>
+      <c r="C33" cm="1">
+        <f t="array" ref="C33">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A33)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-3</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>[-4, -3],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34" cm="1">
+        <f t="array" ref="B34">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A34)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-4</v>
+      </c>
+      <c r="C34" cm="1">
+        <f t="array" ref="C34">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A34)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-5</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>[-4, -5],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35" cm="1">
+        <f t="array" ref="B35">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A35)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-4</v>
+      </c>
+      <c r="C35" cm="1">
+        <f t="array" ref="C35">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A35)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-7</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>[-4, -7],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>13</v>
+      </c>
+      <c r="B36" cm="1">
+        <f t="array" ref="B36">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A36)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-2</v>
+      </c>
+      <c r="C36" cm="1">
+        <f t="array" ref="C36">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A36)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>[-2, 0],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>14</v>
+      </c>
+      <c r="B37" cm="1">
+        <f t="array" ref="B37">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A37)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-2</v>
+      </c>
+      <c r="C37" cm="1">
+        <f t="array" ref="C37">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A37)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-2</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>[-2, -2],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38" cm="1">
+        <f t="array" ref="B38">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A38)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-2</v>
+      </c>
+      <c r="C38" cm="1">
+        <f t="array" ref="C38">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A38)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-4</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>[-2, -4],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>16</v>
+      </c>
+      <c r="B39" cm="1">
+        <f t="array" ref="B39">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A39)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-2</v>
+      </c>
+      <c r="C39" cm="1">
+        <f t="array" ref="C39">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A39)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-6</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>[-2, -6],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>17</v>
+      </c>
+      <c r="B40" cm="1">
+        <f t="array" ref="B40">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A40)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="C40" cm="1">
+        <f t="array" ref="C40">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A40)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>5</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>[0, 5],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>18</v>
+      </c>
+      <c r="B41" cm="1">
+        <f t="array" ref="B41">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A41)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="C41" cm="1">
+        <f t="array" ref="C41">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A41)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>3</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>[0, 3],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>19</v>
+      </c>
+      <c r="B42" cm="1">
+        <f t="array" ref="B42">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A42)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="C42" cm="1">
+        <f t="array" ref="C42">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A42)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>1</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>[0, 1],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43" cm="1">
+        <f t="array" ref="B43">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A43)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="C43" cm="1">
+        <f t="array" ref="C43">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A43)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>[0, -1],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>21</v>
+      </c>
+      <c r="B44" cm="1">
+        <f t="array" ref="B44">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A44)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="C44" cm="1">
+        <f t="array" ref="C44">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A44)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-3</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>[0, -3],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>22</v>
+      </c>
+      <c r="B45" cm="1">
+        <f t="array" ref="B45">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A45)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="C45" cm="1">
+        <f t="array" ref="C45">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A45)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-5</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>[0, -5],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>23</v>
+      </c>
+      <c r="B46" cm="1">
+        <f t="array" ref="B46">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A46)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>2</v>
+      </c>
+      <c r="C46" cm="1">
+        <f t="array" ref="C46">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A46)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>6</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>[2, 6],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>24</v>
+      </c>
+      <c r="B47" cm="1">
+        <f t="array" ref="B47">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A47)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>2</v>
+      </c>
+      <c r="C47" cm="1">
+        <f t="array" ref="C47">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A47)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>4</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>[2, 4],</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>25</v>
+      </c>
+      <c r="B48" cm="1">
+        <f t="array" ref="B48">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A48)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>2</v>
+      </c>
+      <c r="C48" cm="1">
+        <f t="array" ref="C48">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A48)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>2</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>[2, 2],</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>26</v>
+      </c>
+      <c r="B49" cm="1">
+        <f t="array" ref="B49">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A49)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>2</v>
+      </c>
+      <c r="C49" cm="1">
+        <f t="array" ref="C49">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A49)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>[2, 0],</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>27</v>
+      </c>
+      <c r="B50" cm="1">
+        <f t="array" ref="B50">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A50)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>4</v>
+      </c>
+      <c r="C50" cm="1">
+        <f t="array" ref="C50">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A50)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>7</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>[4, 7],</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>28</v>
+      </c>
+      <c r="B51" cm="1">
+        <f t="array" ref="B51">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A51)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>4</v>
+      </c>
+      <c r="C51" cm="1">
+        <f t="array" ref="C51">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A51)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>5</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>[4, 5],</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>29</v>
+      </c>
+      <c r="B52" cm="1">
+        <f t="array" ref="B52">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A52)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>4</v>
+      </c>
+      <c r="C52" cm="1">
+        <f t="array" ref="C52">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A52)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>3</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>[4, 3],</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>30</v>
+      </c>
+      <c r="B53" cm="1">
+        <f t="array" ref="B53">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A53)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>4</v>
+      </c>
+      <c r="C53" cm="1">
+        <f t="array" ref="C53">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A53)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>[4, 1],</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>31</v>
+      </c>
+      <c r="B54" cm="1">
+        <f t="array" ref="B54">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A54)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>4</v>
+      </c>
+      <c r="C54" cm="1">
+        <f t="array" ref="C54">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A54)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>-1</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>[4, -1],</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>32</v>
+      </c>
+      <c r="B55" cm="1">
+        <f t="array" ref="B55">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A55)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>6</v>
+      </c>
+      <c r="C55" cm="1">
+        <f t="array" ref="C55">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A55)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>6</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>[6, 6],</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>33</v>
+      </c>
+      <c r="B56" cm="1">
+        <f t="array" ref="B56">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A56)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>6</v>
+      </c>
+      <c r="C56" cm="1">
+        <f t="array" ref="C56">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A56)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>4</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>[6, 4],</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>34</v>
+      </c>
+      <c r="B57" cm="1">
+        <f t="array" ref="B57">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A57)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>6</v>
+      </c>
+      <c r="C57" cm="1">
+        <f t="array" ref="C57">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A57)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>2</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>[6, 2],</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>35</v>
+      </c>
+      <c r="B58" cm="1">
+        <f t="array" ref="B58">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A58)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>6</v>
+      </c>
+      <c r="C58" cm="1">
+        <f t="array" ref="C58">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A58)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>0</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>[6, 0],</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>36</v>
+      </c>
+      <c r="B59" cm="1">
+        <f t="array" ref="B59">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A59)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>8</v>
+      </c>
+      <c r="C59" cm="1">
+        <f t="array" ref="C59">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A59)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>5</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>[8, 5],</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>37</v>
+      </c>
+      <c r="B60" cm="1">
+        <f t="array" ref="B60">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A60)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>8</v>
+      </c>
+      <c r="C60" cm="1">
+        <f t="array" ref="C60">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A60)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>3</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>[8, 3],</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>38</v>
+      </c>
+      <c r="B61" cm="1">
+        <f t="array" ref="B61">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A61)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>8</v>
+      </c>
+      <c r="C61" cm="1">
+        <f t="array" ref="C61">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A61)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>1</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>[8, 1],</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>39</v>
+      </c>
+      <c r="B62" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B62" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A62)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C62" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C62" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A62)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D62" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>40</v>
+      </c>
+      <c r="B63" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B63" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A63)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C63" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C63" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A63)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D63" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>41</v>
+      </c>
+      <c r="B64" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B64" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A64)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C64" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C64" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A64)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D64" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>42</v>
+      </c>
+      <c r="B65" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B65" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A65)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C65" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C65" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A65)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D65" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>43</v>
+      </c>
+      <c r="B66" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B66" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A66)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C66" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C66" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A66)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D66" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>44</v>
+      </c>
+      <c r="B67" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B67" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A67)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C67" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C67" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A67)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D67" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>45</v>
+      </c>
+      <c r="B68" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B68" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A68)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C68" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C68" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A68)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D68" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>46</v>
+      </c>
+      <c r="B69" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B69" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A69)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C69" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C69" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A69)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D69" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>47</v>
+      </c>
+      <c r="B70" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B70" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A70)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C70" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C70" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A70)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D70" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>48</v>
+      </c>
+      <c r="B71" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B71" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A71)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C71" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C71" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A71)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D71" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>49</v>
+      </c>
+      <c r="B72" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B72" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A72)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C72" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C72" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A72)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D72" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>50</v>
+      </c>
+      <c r="B73" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B73" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A73)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C73" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C73" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A73)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D73" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>51</v>
+      </c>
+      <c r="B74" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B74" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A74)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C74" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C74" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A74)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D74" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>52</v>
+      </c>
+      <c r="B75" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B75" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A75)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C75" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C75" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A75)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D75" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>53</v>
+      </c>
+      <c r="B76" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B76" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A76)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C76" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C76" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A76)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D76" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>54</v>
+      </c>
+      <c r="B77" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B77" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A77)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C77" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C77" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A77)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D77" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>55</v>
+      </c>
+      <c r="B78" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B78" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A78)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C78" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C78" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A78)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D78" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>56</v>
+      </c>
+      <c r="B79" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B79" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A79)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C79" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C79" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A79)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D79" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>57</v>
+      </c>
+      <c r="B80" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B80" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A80)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C80" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C80" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A80)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D80" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>58</v>
+      </c>
+      <c r="B81" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B81" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A81)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C81" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C81" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A81)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D81" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>59</v>
+      </c>
+      <c r="B82" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B82" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A82)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C82" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C82" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A82)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D82" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>60</v>
+      </c>
+      <c r="B83" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B83" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A83)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C83" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C83" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A83)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D83" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>61</v>
+      </c>
+      <c r="B84" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B84" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A84)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C84" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C84" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A84)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D84" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>62</v>
+      </c>
+      <c r="B85" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B85" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A85)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C85" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C85" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A85)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D85" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>63</v>
+      </c>
+      <c r="B86" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B86" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A86)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C86" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C86" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A86)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D86" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>64</v>
+      </c>
+      <c r="B87" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B87" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A87)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C87" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C87" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A87)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D87" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>65</v>
+      </c>
+      <c r="B88" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B88" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A88)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C88" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C88" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A88)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D88" t="e" vm="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>66</v>
+      </c>
+      <c r="B89" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B89" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A89)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C89" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C89" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A89)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D89" t="e" vm="3">
+        <f t="shared" ref="D89:D91" ca="1" si="1">_xlfn.CONCAT("[",B89,", ",C89,"],")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>67</v>
+      </c>
+      <c r="B90" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B90" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A90)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C90" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="C90" ca="1">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A90)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D90" t="e" vm="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>68</v>
+      </c>
+      <c r="B91" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B91" ca="1">INDEX($C$20:$O$20,,_xlfn.LET(_xlpm.x,($C$3:$O$19=A91)*_xlfn.SEQUENCE(,COLUMNS($C$20:$O$20)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C91" cm="1">
+        <f t="array" ref="C91:C107">INDEX($B$3:$B$19,_xlfn.LET(_xlpm.x,($C$3:$O$19=A91)*_xlfn.SEQUENCE(ROWS($B$3:$B$19)),MIN(IF(_xlpm.x&gt;0,_xlpm.x))))</f>
+        <v>8</v>
+      </c>
+      <c r="D91" t="e" vm="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <v>-8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A3:A19"/>
+    <mergeCell ref="C21:O21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDC7B87-5AFA-48DB-8340-3FB9EC7177FD}">
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9775,7 +11535,7 @@
   <dimension ref="A1:O107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="M14" sqref="I6:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>